<commit_message>
Rename site and applied changes
</commit_message>
<xml_diff>
--- a/docs/mejuri-jewellery-products.xlsx
+++ b/docs/mejuri-jewellery-products.xlsx
@@ -5,10 +5,10 @@
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Milestone Projects\Milestone Project 4\MURA\docs\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Milestone Projects\Milestone Project 4\Mejuri\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{96E578A3-5E9F-48BA-8523-415421729D3F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{55564A9C-CCF4-433D-A6EF-EF9BC8FF75A4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{B30A6D57-9F57-4D1E-BF7F-A6BAB861B0F6}"/>
   </bookViews>
@@ -128,9 +128,6 @@
     <t>Our silver bracelets are comes in a jewellery box with a bag and greeting card. It's a great silver jewellery gifts for women of all ages! Give it to lover, wife, mother, girlfriend family,</t>
   </si>
   <si>
-    <t>https://m.media-amazon.com/images/I/716TSANm8qL._AC_SX679_.jpg</t>
-  </si>
-  <si>
     <t>Angelady Infinity Bracelet for Womens, Silver Infinity Bracelets Bangles</t>
   </si>
   <si>
@@ -201,6 +198,9 @@
   </si>
   <si>
     <t>NECK0009.jpg</t>
+  </si>
+  <si>
+    <t>https://m.media-amazon.com/images/I/61OJmtPZjwL._AC_SX522_.jpg</t>
   </si>
 </sst>
 </file>
@@ -210,7 +210,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.0"/>
   </numFmts>
-  <fonts count="7" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -244,13 +244,6 @@
       <family val="2"/>
     </font>
     <font>
-      <u/>
-      <sz val="11"/>
-      <name val="Aptos Narrow"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <sz val="11"/>
       <color rgb="FF0F1111"/>
       <name val="Aptos Narrow"/>
@@ -278,7 +271,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -298,10 +291,7 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
     </xf>
     <xf numFmtId="164" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
@@ -319,13 +309,13 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1" indent="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1" indent="1"/>
     </xf>
   </cellXfs>
@@ -334,44 +324,6 @@
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="8">
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color auto="1"/>
-        <name val="Aptos Narrow"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color auto="1"/>
-        <name val="Aptos Narrow"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
     <dxf>
       <font>
         <b val="0"/>
@@ -471,6 +423,44 @@
       </font>
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color auto="1"/>
+        <name val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color auto="1"/>
+        <name val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
@@ -485,17 +475,17 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{969C685D-088E-4C8E-9777-D7DA43931C34}" name="Table1" displayName="Table1" ref="A1:H12" totalsRowShown="0" headerRowDxfId="0" dataDxfId="1">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{969C685D-088E-4C8E-9777-D7DA43931C34}" name="Table1" displayName="Table1" ref="A1:H12" totalsRowShown="0" headerRowDxfId="7" dataDxfId="6">
   <autoFilter ref="A1:H12" xr:uid="{969C685D-088E-4C8E-9777-D7DA43931C34}"/>
   <tableColumns count="8">
-    <tableColumn id="1" xr3:uid="{A35EAC39-184C-45BB-BE20-C474ACE821BD}" name="SKU" dataDxfId="7"/>
+    <tableColumn id="1" xr3:uid="{A35EAC39-184C-45BB-BE20-C474ACE821BD}" name="SKU" dataDxfId="5"/>
     <tableColumn id="2" xr3:uid="{1054C798-842A-48BD-A630-53D44B2DE93B}" name="Name"/>
     <tableColumn id="3" xr3:uid="{33D66531-DC3D-455E-9B5C-A2028F2D7010}" name="Description"/>
-    <tableColumn id="4" xr3:uid="{C0CFC9EF-C8BF-475D-AFE3-0DF9B34979E9}" name="Price" dataDxfId="6"/>
-    <tableColumn id="5" xr3:uid="{B7FE19EE-A3E5-464F-8979-A51C01B25B11}" name="Category" dataDxfId="5"/>
-    <tableColumn id="6" xr3:uid="{44BA7685-7E9C-4F3C-A574-F00087DD7C69}" name="Rating" dataDxfId="4"/>
-    <tableColumn id="7" xr3:uid="{237DBB62-E9C0-4870-916E-C07E2FBA1D58}" name="Image URL" dataDxfId="3" dataCellStyle="Hyperlink"/>
-    <tableColumn id="8" xr3:uid="{626A8FAC-F8A6-411F-AB2A-5E181C5C4BB0}" name="Image" dataDxfId="2"/>
+    <tableColumn id="4" xr3:uid="{C0CFC9EF-C8BF-475D-AFE3-0DF9B34979E9}" name="Price" dataDxfId="4"/>
+    <tableColumn id="5" xr3:uid="{B7FE19EE-A3E5-464F-8979-A51C01B25B11}" name="Category" dataDxfId="3"/>
+    <tableColumn id="6" xr3:uid="{44BA7685-7E9C-4F3C-A574-F00087DD7C69}" name="Rating" dataDxfId="2"/>
+    <tableColumn id="7" xr3:uid="{237DBB62-E9C0-4870-916E-C07E2FBA1D58}" name="Image URL" dataDxfId="1" dataCellStyle="Hyperlink"/>
+    <tableColumn id="8" xr3:uid="{626A8FAC-F8A6-411F-AB2A-5E181C5C4BB0}" name="Image" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -821,16 +811,15 @@
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:H10"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <pane xSplit="1" topLeftCell="D1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" sqref="A1:H12"/>
+    <sheetView tabSelected="1" topLeftCell="C7" workbookViewId="0">
+      <selection activeCell="G10" sqref="G10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="10" style="3" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="32.7109375" style="3" customWidth="1"/>
-    <col min="3" max="3" width="29" style="12" customWidth="1"/>
+    <col min="3" max="3" width="29" style="11" customWidth="1"/>
     <col min="4" max="4" width="11.5703125" style="3" customWidth="1"/>
     <col min="5" max="5" width="17.42578125" style="3" customWidth="1"/>
     <col min="6" max="6" width="8.85546875" style="3" customWidth="1"/>
@@ -846,7 +835,7 @@
       <c r="B1" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="12" t="s">
+      <c r="C1" s="11" t="s">
         <v>2</v>
       </c>
       <c r="D1" s="3" t="s">
@@ -872,7 +861,7 @@
       <c r="B2" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="C2" s="13" t="s">
+      <c r="C2" s="12" t="s">
         <v>11</v>
       </c>
       <c r="D2" s="5">
@@ -888,17 +877,17 @@
         <v>20</v>
       </c>
       <c r="H2" s="3" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="3" spans="1:8" ht="135" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="B3" s="10" t="s">
+      <c r="B3" s="9" t="s">
         <v>13</v>
       </c>
-      <c r="C3" s="8" t="s">
+      <c r="C3" s="7" t="s">
         <v>15</v>
       </c>
       <c r="D3" s="5">
@@ -907,24 +896,24 @@
       <c r="E3" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="F3" s="9">
+      <c r="F3" s="8">
         <v>4</v>
       </c>
-      <c r="G3" s="7" t="s">
+      <c r="G3" s="1" t="s">
         <v>12</v>
       </c>
       <c r="H3" s="3" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="4" spans="1:8" ht="135" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="B4" s="11" t="s">
+      <c r="B4" s="10" t="s">
         <v>21</v>
       </c>
-      <c r="C4" s="8" t="s">
+      <c r="C4" s="7" t="s">
         <v>15</v>
       </c>
       <c r="D4" s="5">
@@ -940,7 +929,7 @@
         <v>19</v>
       </c>
       <c r="H4" s="3" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="5" spans="1:8" ht="45" x14ac:dyDescent="0.25">
@@ -950,7 +939,7 @@
       <c r="B5" s="6" t="s">
         <v>26</v>
       </c>
-      <c r="C5" s="14" t="s">
+      <c r="C5" s="13" t="s">
         <v>27</v>
       </c>
       <c r="D5" s="5">
@@ -966,7 +955,7 @@
         <v>25</v>
       </c>
       <c r="H5" s="3" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="6" spans="1:8" ht="45" x14ac:dyDescent="0.25">
@@ -976,7 +965,7 @@
       <c r="B6" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="C6" s="14" t="s">
+      <c r="C6" s="13" t="s">
         <v>29</v>
       </c>
       <c r="D6" s="5">
@@ -989,10 +978,10 @@
         <v>4.5999999999999996</v>
       </c>
       <c r="G6" s="1" t="s">
-        <v>30</v>
+        <v>54</v>
       </c>
       <c r="H6" s="3" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="7" spans="1:8" ht="45" x14ac:dyDescent="0.25">
@@ -1000,10 +989,10 @@
         <v>24</v>
       </c>
       <c r="B7" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="C7" s="13" t="s">
         <v>31</v>
-      </c>
-      <c r="C7" s="14" t="s">
-        <v>32</v>
       </c>
       <c r="D7" s="5">
         <v>45</v>
@@ -1015,21 +1004,21 @@
         <v>4.0999999999999996</v>
       </c>
       <c r="G7" s="1" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="H7" s="3" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="8" spans="1:8" ht="150" x14ac:dyDescent="0.25">
       <c r="A8" s="3" t="s">
-        <v>34</v>
-      </c>
-      <c r="B8" s="15" t="s">
+        <v>33</v>
+      </c>
+      <c r="B8" s="14" t="s">
+        <v>36</v>
+      </c>
+      <c r="C8" s="15" t="s">
         <v>37</v>
-      </c>
-      <c r="C8" s="16" t="s">
-        <v>38</v>
       </c>
       <c r="D8" s="5">
         <v>105</v>
@@ -1041,21 +1030,21 @@
         <v>4.5</v>
       </c>
       <c r="G8" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="H8" s="3" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="9" spans="1:8" ht="45" x14ac:dyDescent="0.25">
       <c r="A9" s="3" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B9" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="C9" s="13" t="s">
         <v>40</v>
-      </c>
-      <c r="C9" s="14" t="s">
-        <v>41</v>
       </c>
       <c r="D9" s="5">
         <v>45</v>
@@ -1067,21 +1056,21 @@
         <v>4.2</v>
       </c>
       <c r="G9" s="1" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="H9" s="3" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="10" spans="1:8" ht="45" x14ac:dyDescent="0.25">
       <c r="A10" s="3" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B10" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="C10" s="13" t="s">
         <v>43</v>
-      </c>
-      <c r="C10" s="14" t="s">
-        <v>44</v>
       </c>
       <c r="D10" s="5">
         <v>85</v>
@@ -1093,10 +1082,10 @@
         <v>4.9000000000000004</v>
       </c>
       <c r="G10" s="1" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="H10" s="3" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
   </sheetData>

</xml_diff>